<commit_message>
Implimented the logic in process
</commit_message>
<xml_diff>
--- a/Input/Data.xlsx
+++ b/Input/Data.xlsx
@@ -1,33 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2025.01\Workflows\Input\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A0A313-FDE3-4A40-8B3D-DFCE38455E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$11</definedName>
-  </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="20">
   <si>
     <t>Sr.
 No</t>
@@ -42,6 +40,12 @@
     <t>RRN</t>
   </si>
   <si>
+    <t>Macro Name</t>
+  </si>
+  <si>
+    <t>Number of Matches</t>
+  </si>
+  <si>
     <t>UPI</t>
   </si>
   <si>
@@ -51,40 +55,43 @@
     <t>Yes</t>
   </si>
   <si>
+    <t xml:space="preserve">            Wallet:: refunded - ARN/PRN available - 1st response_UPI - PPBL , Remitter - PPBL            Wallet:: refunded - ARN/PRN available - 1st response_UPI - PPBL , Remitter - PPBL            Wallet:: refunded - ARN/PRN available - 1st response_UPI - PPBL , Remitter - PPBL            Wallet:: refunded - ARN/PRN available - 1st response_UPI - PPBL , Remitter - PPBL            Wallet:: refunded - ARN/PRN available - 1st response_UPI - PPBL , Remitter - PPBL            Wallet:: refunded - ARN/PRN available - 1st response_UPI - PPBL , Remitter - PPBL</t>
+  </si>
+  <si>
+    <t>SBI</t>
+  </si>
+  <si>
     <t>No</t>
   </si>
   <si>
+    <t xml:space="preserve">            Wallet:: ARN/PRN not available - 1st response_UPI - PPBL, Remitter - PPBL            Wallet:: ARN/PRN not available - 1st response_UPI - PPBL, Remitter - PPBL            Wallet:: ARN/PRN not available - 1st response_UPI - PPBL, Remitter - PPBL            Wallet:: ARN/PRN not available - 1st response_UPI - PPBL, Remitter - PPBL            Wallet:: ARN/PRN not available - 1st response_UPI - PPBL, Remitter - PPBL            Wallet:: ARN/PRN not available - 1st response_UPI - PPBL, Remitter - PPBL            Wallet:: Refunded - ARN/PRN available - 1st response_Non PPBL</t>
+  </si>
+  <si>
     <t>NB</t>
   </si>
   <si>
+    <t xml:space="preserve">            Wallet:: Refunded - ARN/PRN available - 1st response_Non PPBL</t>
+  </si>
+  <si>
     <t>CC</t>
   </si>
   <si>
+    <t>Corporation Bank</t>
+  </si>
+  <si>
     <t>DC</t>
   </si>
   <si>
-    <t>SBI</t>
-  </si>
-  <si>
-    <t>Corporation Bank</t>
-  </si>
-  <si>
     <t>HDFC</t>
   </si>
   <si>
     <t>ICICI</t>
-  </si>
-  <si>
-    <t>Macro Name</t>
-  </si>
-  <si>
-    <t>Number of Matches</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -128,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -137,9 +144,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -448,31 +452,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" activeCellId="5" sqref="C3 C5 C8 C9 C10 C11"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -486,150 +490,210 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>